<commit_message>
rename birthday to birthdate
</commit_message>
<xml_diff>
--- a/app/config/tables/eonasdan/forms/eonasdan/eonasdan.xlsx
+++ b/app/config/tables/eonasdan/forms/eonasdan/eonasdan.xlsx
@@ -141,13 +141,13 @@
     <t>display.title.text</t>
   </si>
   <si>
-    <t>birthday</t>
-  </si>
-  <si>
     <t>example0</t>
   </si>
   <si>
     <t>Birthday</t>
+  </si>
+  <si>
+    <t>birthdate</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,7 +355,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,7 +567,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,14 +650,14 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>

</xml_diff>